<commit_message>
dsa topological sort and js
</commit_message>
<xml_diff>
--- a/java/Mixed_Review.xlsx
+++ b/java/Mixed_Review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64539E4E-9BFB-44FA-A6E5-8E97F1D47014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0314D770-1A83-43BD-94B6-6E3FFC665617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
   <si>
     <t>Question</t>
   </si>
@@ -222,6 +222,18 @@
   </si>
   <si>
     <t>Use a stack. Upon '(' push the curr score and enter the next inner layer level, reset cur = 0. If ')' is encountered, cur score is doubled and is atleast 1. Exit the curr layer level, set cur += stack.pop() + cur. For O(1) you need to change the array and pointer approach and count the layers.</t>
+  </si>
+  <si>
+    <t>2115. Find All Possible Recipes from Given Supplies</t>
+  </si>
+  <si>
+    <t>Topological Sort</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/find-all-possible-recipes-from-given-supplies/solutions/1646584/java-python-3-toplogical-sort-w-brief-explanation/ </t>
+  </si>
+  <si>
+    <t>Brute force is repeated BFS. Optimal is Topological Sort. For each recipe, count of its dependent ingredients as degree, and store (ingredient, recipes that depend on it) as HashMap. Use supplies as the starting points of the topological sort. Use top sort to decrease the in degree of recipes, when in degree reaches 0, add to return list.</t>
   </si>
 </sst>
 </file>
@@ -332,8 +344,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E16" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E16" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E17" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E17" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{39CFF8EE-B425-4749-92A0-090E902A657C}" name="Question"/>
     <tableColumn id="2" xr3:uid="{818806AE-0CAD-47D4-9900-447AC000C09C}" name="Difficulty" dataDxfId="0"/>
@@ -608,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,6 +905,23 @@
       </c>
       <c r="E16" s="2" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -912,11 +941,12 @@
     <hyperlink ref="E14" r:id="rId13" xr:uid="{C000C4B8-FB1D-41F8-A869-F7C307B6EA77}"/>
     <hyperlink ref="E15" r:id="rId14" xr:uid="{F12AB4DF-4DF1-4FF5-89CD-8F921C3BAC03}"/>
     <hyperlink ref="E16" r:id="rId15" xr:uid="{90BBF423-D96F-4D61-847A-DCE6B07B9EFD}"/>
+    <hyperlink ref="E17" r:id="rId16" xr:uid="{3F12C46F-A472-47C6-892B-FF69CA6B4DBA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
   <tableParts count="1">
-    <tablePart r:id="rId17"/>
+    <tablePart r:id="rId18"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dsa dp and js
</commit_message>
<xml_diff>
--- a/java/Mixed_Review.xlsx
+++ b/java/Mixed_Review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0314D770-1A83-43BD-94B6-6E3FFC665617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF3A292-F88C-42ED-9965-2694EE8977A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="69">
   <si>
     <t>Question</t>
   </si>
@@ -234,6 +234,15 @@
   </si>
   <si>
     <t>Brute force is repeated BFS. Optimal is Topological Sort. For each recipe, count of its dependent ingredients as degree, and store (ingredient, recipes that depend on it) as HashMap. Use supplies as the starting points of the topological sort. Use top sort to decrease the in degree of recipes, when in degree reaches 0, add to return list.</t>
+  </si>
+  <si>
+    <t>403. Frog Jump</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/frog-jump/solutions/193816/concise-and-fast-dp-solution-using-2d-array-instead-of-hashmap-with-text-and-video-explanation/</t>
+  </si>
+  <si>
+    <t>Calculate the reach based on the distances of the stones until the end and see if the final stone can be reached. We can use a HashMap with a HashSet of steps at each stone, or a 2D array DP.</t>
   </si>
 </sst>
 </file>
@@ -344,8 +353,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E17" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E17" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E18" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E18" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{39CFF8EE-B425-4749-92A0-090E902A657C}" name="Question"/>
     <tableColumn id="2" xr3:uid="{818806AE-0CAD-47D4-9900-447AC000C09C}" name="Difficulty" dataDxfId="0"/>
@@ -620,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,6 +931,23 @@
       </c>
       <c r="E17" s="2" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -942,11 +968,12 @@
     <hyperlink ref="E15" r:id="rId14" xr:uid="{F12AB4DF-4DF1-4FF5-89CD-8F921C3BAC03}"/>
     <hyperlink ref="E16" r:id="rId15" xr:uid="{90BBF423-D96F-4D61-847A-DCE6B07B9EFD}"/>
     <hyperlink ref="E17" r:id="rId16" xr:uid="{3F12C46F-A472-47C6-892B-FF69CA6B4DBA}"/>
+    <hyperlink ref="E18" r:id="rId17" xr:uid="{554071B2-E339-4D90-8EF3-472E042EAB44}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
   <tableParts count="1">
-    <tablePart r:id="rId18"/>
+    <tablePart r:id="rId19"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
lc ll and trees
</commit_message>
<xml_diff>
--- a/java/Mixed_Review.xlsx
+++ b/java/Mixed_Review.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F92433B-AC7F-4638-B32D-9B8E93375C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1501535-A92F-4F04-BCA6-6AFB1B474EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="110">
   <si>
     <t>Question</t>
   </si>
@@ -345,6 +345,27 @@
   </si>
   <si>
     <t xml:space="preserve">https://leetcode.com/problems/merge-intervals/solutions/5097671/java-easy-to-understand-solution-with-explanation/ </t>
+  </si>
+  <si>
+    <t>19. Remove Nth Node From End of List</t>
+  </si>
+  <si>
+    <t>Linked List</t>
+  </si>
+  <si>
+    <t>Maintain a pointer to the head. Create a dummy node to iterate first, n ahead of the tail, so you can check for null nodes with a while loop. Then just set tail.next to dummy.next, then return head.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/remove-nth-node-from-end-of-list/solutions/5121069/video-using-distance-between-two-pointers/ </t>
+  </si>
+  <si>
+    <t>102. Binary Tree Level Order Trabersal</t>
+  </si>
+  <si>
+    <t>Use BFS traversal of a binary tree. Maintain both a res list and a level list and watch out for the null head case.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/binary-tree-level-order-traversal/solutions/3267417/well-explained-code-in-java-use-of-arraylist-and-queues/ </t>
   </si>
 </sst>
 </file>
@@ -455,8 +476,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E28" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E28" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}" name="Table2" displayName="Table2" ref="A1:E30" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E30" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{39CFF8EE-B425-4749-92A0-090E902A657C}" name="Question"/>
     <tableColumn id="2" xr3:uid="{818806AE-0CAD-47D4-9900-447AC000C09C}" name="Difficulty" dataDxfId="0"/>
@@ -731,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1220,6 +1241,40 @@
       </c>
       <c r="E28" s="2" t="s">
         <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" t="s">
+        <v>104</v>
+      </c>
+      <c r="D29" t="s">
+        <v>105</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>107</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" t="s">
+        <v>108</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1251,11 +1306,13 @@
     <hyperlink ref="E26" r:id="rId25" xr:uid="{A0D0E7E1-B5B0-4038-A1FE-7724CF45C4DF}"/>
     <hyperlink ref="E27" r:id="rId26" xr:uid="{4E8A8BD6-777A-44A8-8029-C838EBDB9950}"/>
     <hyperlink ref="E28" r:id="rId27" xr:uid="{BBCF1EBB-F9C0-4FAB-A29C-E0E89141F10D}"/>
+    <hyperlink ref="E29" r:id="rId28" xr:uid="{3325A7DE-690D-4262-8984-85DC4ED4C15F}"/>
+    <hyperlink ref="E30" r:id="rId29" xr:uid="{52444B81-2EE9-4677-8017-675A49E2CC1D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId28"/>
+  <pageSetup orientation="portrait" r:id="rId30"/>
   <tableParts count="1">
-    <tablePart r:id="rId29"/>
+    <tablePart r:id="rId31"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dsa dp and cpp
</commit_message>
<xml_diff>
--- a/java/Mixed_Review.xlsx
+++ b/java/Mixed_Review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF7D30DA-989D-47D6-898C-8CE438F3EB5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C7B9D5-5247-4124-83FC-EE832AEEA15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="145">
   <si>
     <t>Question</t>
   </si>
@@ -457,6 +457,21 @@
   </si>
   <si>
     <t>Optimal is 1 pass with complement hashtable.</t>
+  </si>
+  <si>
+    <t>Two Pointers</t>
+  </si>
+  <si>
+    <t>121. Best Time to Buy and Sell Stock</t>
+  </si>
+  <si>
+    <t>Kadane's is optimal,  but 2 pointers is best for intereview setting. Updating least so far is also intuitive.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/best-time-to-buy-and-sell-stock/solutions/1735493/java-c-best-ever-explanation-could-possible/ </t>
+  </si>
+  <si>
+    <t>Remember the recursive relation argmax(dfs(i-2) + curr, dfs(i-1)).</t>
   </si>
 </sst>
 </file>
@@ -594,8 +609,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0889DD6-65BF-4CF4-A25E-553A3E1C807F}" name="Table22" displayName="Table22" ref="A1:E2" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E2" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0889DD6-65BF-4CF4-A25E-553A3E1C807F}" name="Table22" displayName="Table22" ref="A1:E4" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E4" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{48BE1778-7CDA-4ED7-830C-FBF7CEC5F641}" name="Question"/>
     <tableColumn id="2" xr3:uid="{BB2891EA-9253-4017-A45F-1AE59DC7D5B3}" name="Difficulty" dataDxfId="0"/>
@@ -1581,17 +1596,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C3D48E0-4D21-4751-ABF7-460D56FF37CF}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="62.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="165" bestFit="1" customWidth="1"/>
   </cols>
@@ -1630,11 +1645,49 @@
         <v>138</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{3F490A31-5AB1-4485-AEC8-D9DAADB8AED5}"/>
+    <hyperlink ref="E4" r:id="rId2" xr:uid="{6F07B1F3-B91B-454D-A5F9-3449B38DB3B0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
c++ hashing, java trees
</commit_message>
<xml_diff>
--- a/java/Mixed_Review.xlsx
+++ b/java/Mixed_Review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15AD586-13A0-4ADC-9615-68113B2142AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249DA5E9-AAA4-4ABC-8912-FF0A887F1271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="156">
   <si>
     <t>Question</t>
   </si>
@@ -477,9 +477,6 @@
     <t xml:space="preserve">https://leetcode.com/problems/reverse-linked-list/solutions/58125/in-place-iterative-and-recursive-java-solution/ </t>
   </si>
   <si>
-    <t>Recursive relation argmax(dfs(i-2) + curr, dfs(i-1)).</t>
-  </si>
-  <si>
     <t>LL traversal and manipulation template. Remembering the recursive solution is helpful for later.</t>
   </si>
   <si>
@@ -487,6 +484,27 @@
   </si>
   <si>
     <t>DFS &gt; Top-down memo &gt; Bottom-up DP &gt; Reach solution. Analysis</t>
+  </si>
+  <si>
+    <t>Recursive relation argmax(dfs(i-2) + curr, dfs(i-1)). Fibonacci is Optimal.</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/invert-binary-tree/solutions/62707/straightforward-dfs-recursive-iterative-bfs-solutions/</t>
+  </si>
+  <si>
+    <t>Recursive DFS &gt; Stack &gt; Iterative BFS (Level Order Traversal)</t>
+  </si>
+  <si>
+    <t>226. Invert Binary Tree</t>
+  </si>
+  <si>
+    <t>104. Maximum Depth of Binary Tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/maximum-depth-of-binary-tree/solutions/1770060/c-recursive-dfs-example-dry-run-well-explained/ </t>
+  </si>
+  <si>
+    <t>Recursive DFS of both sides, and recursive relation of max(maxL, maxR)+1;</t>
   </si>
 </sst>
 </file>
@@ -624,8 +642,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0889DD6-65BF-4CF4-A25E-553A3E1C807F}" name="Table22" displayName="Table22" ref="A1:E6" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E6" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0889DD6-65BF-4CF4-A25E-553A3E1C807F}" name="Table22" displayName="Table22" ref="A1:E8" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E8" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{48BE1778-7CDA-4ED7-830C-FBF7CEC5F641}" name="Question"/>
     <tableColumn id="2" xr3:uid="{BB2891EA-9253-4017-A45F-1AE59DC7D5B3}" name="Difficulty" dataDxfId="0"/>
@@ -1611,10 +1629,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C3D48E0-4D21-4751-ABF7-460D56FF37CF}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1688,7 +1706,7 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>131</v>
@@ -1705,7 +1723,7 @@
         <v>104</v>
       </c>
       <c r="D5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>145</v>
@@ -1722,10 +1740,44 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>151</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>155</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -1734,11 +1786,12 @@
     <hyperlink ref="E4" r:id="rId2" xr:uid="{6F07B1F3-B91B-454D-A5F9-3449B38DB3B0}"/>
     <hyperlink ref="E5" r:id="rId3" xr:uid="{2115C330-82FA-4BD8-8739-C97FBF177386}"/>
     <hyperlink ref="E6" r:id="rId4" xr:uid="{3B2E9035-D82F-42A4-84AA-F23669231012}"/>
+    <hyperlink ref="E8" r:id="rId5" xr:uid="{C9470CED-E83D-4B9E-9DFA-BB1F50A606EF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dsa backtracking and stacks
</commit_message>
<xml_diff>
--- a/java/Mixed_Review.xlsx
+++ b/java/Mixed_Review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8809528B-68E6-4FB1-9A5F-9455D0080830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{653A23BE-EEDC-4243-B85E-9710A9BD093E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="177">
   <si>
     <t>Question</t>
   </si>
@@ -559,6 +559,15 @@
   </si>
   <si>
     <t>Base case is amount remain = 0 then 0, and amount &lt; 0 then return -1 invalid. We are getting the remainder at each step and looking for a solution with a 0 remainder exactly. Recursive relation ship is count = coinCount(coins, amount - coins[i]). Then maintain and update minCoins = min(minCoins, 1 + count).</t>
+  </si>
+  <si>
+    <t>Classic Stack, only need to maintain order in this one. Can do push complement method.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/valid-parentheses/solutions/9178/short-java-solution/ </t>
+  </si>
+  <si>
+    <t>Use a void backtrack function. Start from index 1. Remember the base case and passing new list in function argument, and iterating both k and I in the recursion. Remember the take and not take with .add() and .remove() of the current list.</t>
   </si>
 </sst>
 </file>
@@ -1685,8 +1694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C3D48E0-4D21-4751-ABF7-460D56FF37CF}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1946,7 +1955,12 @@
       <c r="C15" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="2"/>
+      <c r="D15" t="s">
+        <v>176</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1958,7 +1972,12 @@
       <c r="C16" t="s">
         <v>53</v>
       </c>
-      <c r="E16" s="2"/>
+      <c r="D16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>175</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1973,11 +1992,13 @@
     <hyperlink ref="E12" r:id="rId9" xr:uid="{BDA469E2-DFCB-44C9-8807-CD5999379FA8}"/>
     <hyperlink ref="E13" r:id="rId10" xr:uid="{6A001D82-4756-48FF-983A-3105D3B99AD1}"/>
     <hyperlink ref="E14" r:id="rId11" xr:uid="{C8499DE6-5EC7-460B-9274-46A687B889DC}"/>
+    <hyperlink ref="E16" r:id="rId12" xr:uid="{650DDB33-C393-49EF-8B67-46346D715E0F}"/>
+    <hyperlink ref="E15" r:id="rId13" xr:uid="{92CBE994-F4E6-4B50-9C8A-E701D531A9F3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
   <tableParts count="1">
-    <tablePart r:id="rId13"/>
+    <tablePart r:id="rId15"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
lc practice stacks, ll, recursion
</commit_message>
<xml_diff>
--- a/java/Mixed_Review.xlsx
+++ b/java/Mixed_Review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF5A120-C145-4BF8-8A7C-05AFF62C27EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{613D5F20-3B87-4CA7-8085-3AD16B3546BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="220">
   <si>
     <t>Question</t>
   </si>
@@ -588,9 +588,6 @@
     <t xml:space="preserve">https://leetcode.com/problems/subarray-with-elements-greater-than-varying-threshold/solutions/2260048/java-solution-using-monotonic-stack-with-explanation/?envType=company&amp;envId=tiktok&amp;favoriteSlug=tiktok-thirty-days </t>
   </si>
   <si>
-    <t>Monotonic Stack for min element of each subarray and length of subarray. Brute force way is to create all subarrays.</t>
-  </si>
-  <si>
     <t>1647. Minimum Deletions to Make Character Frequencies Unique</t>
   </si>
   <si>
@@ -688,6 +685,18 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/remove-duplicate-letters/solutions/1859410/java-c-detailed-visually-explained/?envType=company&amp;envId=bytedance&amp;favoriteSlug=bytedance-thirty-days</t>
+  </si>
+  <si>
+    <t>Monotonic Stack for min element of each subarray and length of subarray. Brute force way is to create all subarrays. Alternatively, Recursion is a good solution.</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/lru-cache/solutions/45911/java-hashtable-double-linked-list-with-a-touch-of-pseudo-nodes/?envType=company&amp;envId=bytedance&amp;favoriteSlug=bytedance-thirty-days</t>
+  </si>
+  <si>
+    <t>Need to use Hash table and a Doubly Linked List. OOP and DS implementation.</t>
+  </si>
+  <si>
+    <t>Use char freq map + a stack.</t>
   </si>
 </sst>
 </file>
@@ -1814,8 +1823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C3D48E0-4D21-4751-ABF7-460D56FF37CF}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2144,7 +2153,7 @@
         <v>53</v>
       </c>
       <c r="D19" t="s">
-        <v>183</v>
+        <v>216</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>182</v>
@@ -2152,7 +2161,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>11</v>
@@ -2161,15 +2170,15 @@
         <v>137</v>
       </c>
       <c r="D20" t="s">
+        <v>188</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>189</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>5</v>
@@ -2178,10 +2187,10 @@
         <v>100</v>
       </c>
       <c r="D21" t="s">
+        <v>199</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2195,15 +2204,15 @@
         <v>100</v>
       </c>
       <c r="D22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>11</v>
@@ -2212,15 +2221,15 @@
         <v>100</v>
       </c>
       <c r="D23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>11</v>
@@ -2229,7 +2238,7 @@
         <v>53</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2243,15 +2252,15 @@
         <v>111</v>
       </c>
       <c r="D25" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>11</v>
@@ -2260,15 +2269,15 @@
         <v>111</v>
       </c>
       <c r="D26" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>11</v>
@@ -2277,16 +2286,24 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="2"/>
+      <c r="C28" t="s">
+        <v>104</v>
+      </c>
+      <c r="D28" t="s">
+        <v>218</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>11</v>
@@ -2294,13 +2311,16 @@
       <c r="C29" t="s">
         <v>53</v>
       </c>
+      <c r="D29" t="s">
+        <v>219</v>
+      </c>
       <c r="E29" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>11</v>
@@ -2312,7 +2332,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>11</v>
@@ -2321,7 +2341,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>11</v>
@@ -2330,7 +2350,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>5</v>
@@ -2348,10 +2368,10 @@
         <v>37</v>
       </c>
       <c r="D34" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -2365,15 +2385,15 @@
         <v>104</v>
       </c>
       <c r="D35" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>11</v>
@@ -2382,7 +2402,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>11</v>
@@ -2391,7 +2411,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
dsa binary search and lru cache
</commit_message>
<xml_diff>
--- a/java/Mixed_Review.xlsx
+++ b/java/Mixed_Review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73DF40C4-D53D-4C36-BC71-235844DED09D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795A2BEC-D913-4005-9C32-E2EDB32AD5DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="228">
   <si>
     <t>Question</t>
   </si>
@@ -687,12 +687,6 @@
     <t>Monotonic Stack for min element of each subarray and length of subarray. Brute force way is to create all subarrays. Alternatively, Recursion is a good solution.</t>
   </si>
   <si>
-    <t>https://leetcode.com/problems/lru-cache/solutions/45911/java-hashtable-double-linked-list-with-a-touch-of-pseudo-nodes/?envType=company&amp;envId=bytedance&amp;favoriteSlug=bytedance-thirty-days</t>
-  </si>
-  <si>
-    <t>Need to use Hash table and a Doubly Linked List. OOP and DS implementation.</t>
-  </si>
-  <si>
     <t>Use char freq map + a stack.</t>
   </si>
   <si>
@@ -715,6 +709,18 @@
   </si>
   <si>
     <t xml:space="preserve"> https://leetcode.com/problems/first-day-where-you-have-been-in-all-the-rooms/solutions/1459388/understanding-the-logic/ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/sqrtx/ </t>
+  </si>
+  <si>
+    <t>Binary search or Newton's method. The trick is to look in i &lt;= x/i to avoid integer upper limit. Look for the critical point: mid == x/mid.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/lru-cache/solutions/3780815/dll-map-c-java-python-beginner-friendly/ </t>
+  </si>
+  <si>
+    <t>1. extend LinkedHashMap. 2. Manual Implementation: Need to use HashMap and a Doubly Linked List. Need DLL Node, HashMap&lt;Integer, Node&gt;, and addNode() and deleteNode() functions.</t>
   </si>
 </sst>
 </file>
@@ -1841,8 +1847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C3D48E0-4D21-4751-ABF7-460D56FF37CF}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2304,10 +2310,10 @@
         <v>37</v>
       </c>
       <c r="D27" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2321,10 +2327,10 @@
         <v>104</v>
       </c>
       <c r="D28" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2338,7 +2344,7 @@
         <v>53</v>
       </c>
       <c r="D29" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>214</v>
@@ -2355,10 +2361,10 @@
         <v>53</v>
       </c>
       <c r="D30" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2372,10 +2378,10 @@
         <v>12</v>
       </c>
       <c r="D31" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2394,7 +2400,15 @@
       <c r="B33" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E33" s="2"/>
+      <c r="C33" t="s">
+        <v>115</v>
+      </c>
+      <c r="D33" t="s">
+        <v>225</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -2407,7 +2421,7 @@
         <v>37</v>
       </c>
       <c r="D34" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>212</v>
@@ -2486,11 +2500,13 @@
     <hyperlink ref="E29" r:id="rId22" xr:uid="{E485FCF0-3E47-4BC7-A588-8E9961F48ADD}"/>
     <hyperlink ref="E27" r:id="rId23" xr:uid="{27D4F870-2C50-47BA-9AA7-56B35E548864}"/>
     <hyperlink ref="E30" r:id="rId24" xr:uid="{0058F758-48A3-4BCF-A6C4-0491CF44DFB3}"/>
+    <hyperlink ref="E33" r:id="rId25" xr:uid="{AEB4740E-F9BB-4AB7-9AFC-3D9A4BC1BE14}"/>
+    <hyperlink ref="E28" r:id="rId26" xr:uid="{FE51583E-9454-41F4-AFD4-3CBEFC7A97D3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId25"/>
+  <pageSetup orientation="portrait" r:id="rId27"/>
   <tableParts count="1">
-    <tablePart r:id="rId26"/>
+    <tablePart r:id="rId28"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
selenium research database scrapers
</commit_message>
<xml_diff>
--- a/java/Mixed_Review.xlsx
+++ b/java/Mixed_Review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D9C27C-C115-4F21-8084-1ABB6D254FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB3BEFF6-0A94-45FC-90E8-4C24AD1B2593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="244">
   <si>
     <t>Question</t>
   </si>
@@ -766,6 +766,9 @@
   </si>
   <si>
     <t>Use a stack. Push positives, and deal with negative current asteroid cases. At the end fill the res arr from the stack.</t>
+  </si>
+  <si>
+    <t>503. Next Greater Element 2</t>
   </si>
 </sst>
 </file>
@@ -903,8 +906,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0889DD6-65BF-4CF4-A25E-553A3E1C807F}" name="Table22" displayName="Table22" ref="A1:E40" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E40" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0889DD6-65BF-4CF4-A25E-553A3E1C807F}" name="Table22" displayName="Table22" ref="A1:E41" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E41" xr:uid="{8A5E5259-EAE7-4B70-A567-E3F2ADB589C1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{48BE1778-7CDA-4ED7-830C-FBF7CEC5F641}" name="Question"/>
     <tableColumn id="2" xr3:uid="{BB2891EA-9253-4017-A45F-1AE59DC7D5B3}" name="Difficulty" dataDxfId="0"/>
@@ -1890,10 +1893,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C3D48E0-4D21-4751-ABF7-460D56FF37CF}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2576,6 +2579,18 @@
       <c r="E40" s="2" t="s">
         <v>239</v>
       </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>243</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" t="s">
+        <v>53</v>
+      </c>
+      <c r="E41" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>